<commit_message>
Summary Dashboard finished. Created more measures, columns, field parameters, groups etc. Begun the Overview dashboard with trend analysis and State analysis charts finished
</commit_message>
<xml_diff>
--- a/Variables in the dashboard.xlsx
+++ b/Variables in the dashboard.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gangu\OneDrive\Desktop\Academics\Bank Loan Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2862F52F-5590-43AC-BAB5-6E9D34EF2986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092F7E6F-6992-4443-9302-AC7631A123ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Measures" sheetId="1" r:id="rId1"/>
     <sheet name="table" sheetId="2" r:id="rId2"/>
-    <sheet name="column" sheetId="3" r:id="rId3"/>
+    <sheet name="new columns" sheetId="3" r:id="rId3"/>
     <sheet name="Groups" sheetId="4" r:id="rId4"/>
+    <sheet name="Field parameter" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>total_loan_applications</t>
   </si>
@@ -93,10 +94,58 @@
     <t>date_table</t>
   </si>
   <si>
-    <t>month column in table date</t>
-  </si>
-  <si>
     <t>Good v Bad Loans</t>
+  </si>
+  <si>
+    <t>Good Loan %</t>
+  </si>
+  <si>
+    <t>Good Loan Applications</t>
+  </si>
+  <si>
+    <t>Good Loan Funded Amount</t>
+  </si>
+  <si>
+    <t>Good Loan Amount Received</t>
+  </si>
+  <si>
+    <t>Bad Loan %</t>
+  </si>
+  <si>
+    <t>Bad Loan Applications</t>
+  </si>
+  <si>
+    <t>Bad Loan Funded Amount</t>
+  </si>
+  <si>
+    <t>Bad Loan Amount Received</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Columns</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>month_number</t>
+  </si>
+  <si>
+    <t>Select Parameter</t>
+  </si>
+  <si>
+    <t>Total Loan Application</t>
+  </si>
+  <si>
+    <t>Total Funded Amount</t>
+  </si>
+  <si>
+    <t>Total Received Amount</t>
   </si>
 </sst>
 </file>
@@ -414,9 +463,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:A28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -518,6 +567,46 @@
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -547,6 +636,42 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9172975E-3994-4E6F-9407-69D2360E6F85}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DC9285C-249B-4DB1-ADEE-FAF71F6596AD}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -565,19 +690,33 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DC9285C-249B-4DB1-ADEE-FAF71F6596AD}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC7178BE-4CC7-48C0-9A53-B56C73EC792B}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>